<commit_message>
Updates? To MY builder?! Impossible! ...
Added selecting all possible spells for Calculator.
</commit_message>
<xml_diff>
--- a/Assets/Exports/BOF III.xlsx
+++ b/Assets/Exports/BOF III.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
   <si>
     <t>Ryu</t>
   </si>
@@ -79,7 +79,7 @@
     <t>Dragon Spirit</t>
   </si>
   <si>
-    <t>Counter Magic</t>
+    <t>Speed Save</t>
   </si>
   <si>
     <t>Regenerator</t>
@@ -88,9 +88,6 @@
     <t>Counter</t>
   </si>
   <si>
-    <t>Speed Save</t>
-  </si>
-  <si>
     <t>Move +3</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
     <t>Gained JP Up: (Squire - 250 JP)</t>
   </si>
   <si>
+    <t>Accumulate: (Squire - 300 JP)</t>
+  </si>
+  <si>
     <t>Move +1: (Squire - 200 JP)</t>
   </si>
   <si>
@@ -190,7 +190,7 @@
     <t>3 Knight</t>
   </si>
   <si>
-    <t>Counter Magic: (Wizard - 800 JP)</t>
+    <t>4 Wizard</t>
   </si>
   <si>
     <t>Regenerator: (Priest - 400 JP)</t>
@@ -205,7 +205,7 @@
     <t>4 Monk</t>
   </si>
   <si>
-    <t>4 Wizard</t>
+    <t>Master Time Mage! (5,300 JP)</t>
   </si>
   <si>
     <t>2 Priest</t>
@@ -217,7 +217,7 @@
     <t>2 Archer</t>
   </si>
   <si>
-    <t>Master Time Mage! (5,300 JP)</t>
+    <t>3 Time Mage</t>
   </si>
   <si>
     <t>Defense Up: (Oracle - 400 JP)</t>
@@ -226,10 +226,10 @@
     <t>3 Archer</t>
   </si>
   <si>
-    <t>2 Thief</t>
-  </si>
-  <si>
-    <t>3 Time Mage</t>
+    <t>3 Thief</t>
+  </si>
+  <si>
+    <t>Master Oracle! (4,670 JP)</t>
   </si>
   <si>
     <t>Move +2: (Thief - 520 JP)</t>
@@ -241,7 +241,7 @@
     <t>Dragon Spirit: (Lancer - 560 JP)</t>
   </si>
   <si>
-    <t>Master Oracle! (4,670 JP)</t>
+    <t>3 Oracle</t>
   </si>
   <si>
     <t>2 Oracle</t>
@@ -250,7 +250,7 @@
     <t>2 Lancer</t>
   </si>
   <si>
-    <t>3 Oracle</t>
+    <t>Master Calculator! (2,550 JP)</t>
   </si>
   <si>
     <t>Master Mediator! (2,200 JP)</t>
@@ -259,9 +259,6 @@
     <t>Two Hands: (Samurai - 900 JP)</t>
   </si>
   <si>
-    <t>Master Calculator! (2,550 JP)</t>
-  </si>
-  <si>
     <t>2 Geomancer</t>
   </si>
   <si>
@@ -274,15 +271,15 @@
     <t>4 Mediator</t>
   </si>
   <si>
+    <t>Master Thief! (2,660 JP)</t>
+  </si>
+  <si>
+    <t>Move +3: (Bard - 1,000 JP)</t>
+  </si>
+  <si>
     <t>4 Geomancer</t>
   </si>
   <si>
-    <t>Master Thief! (2,660 JP)</t>
-  </si>
-  <si>
-    <t>Move +3: (Bard - 1,000 JP)</t>
-  </si>
-  <si>
     <t>Master Knight! (2,400 JP)</t>
   </si>
   <si>
@@ -293,6 +290,15 @@
   </si>
   <si>
     <t>Master Lancer! (5,400 JP)</t>
+  </si>
+  <si>
+    <t>Ice: (Wizard - 50 JP)</t>
+  </si>
+  <si>
+    <t>Ice 2: (Wizard - 200 JP)</t>
+  </si>
+  <si>
+    <t>Ice 3: (Wizard - 480 JP)</t>
   </si>
 </sst>
 </file>
@@ -657,7 +663,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScale="100" view="normal"/>
   </sheetViews>
@@ -760,27 +766,27 @@
         <v>23</v>
       </c>
       <c r="Q6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
         <v>25</v>
       </c>
-      <c r="E7" t="s">
+      <c r="H7" t="s">
         <v>26</v>
       </c>
-      <c r="H7" t="s">
+      <c r="K7" t="s">
+        <v>24</v>
+      </c>
+      <c r="N7" t="s">
         <v>27</v>
       </c>
-      <c r="K7" t="s">
-        <v>25</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="Q7" t="s">
         <v>28</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="9">
@@ -788,37 +794,37 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10">
@@ -826,37 +832,37 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11">
@@ -864,37 +870,37 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12">
@@ -902,37 +908,37 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13">
@@ -940,37 +946,37 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14">
@@ -978,37 +984,37 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="M14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="P14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q14" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15">
@@ -1016,37 +1022,37 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D15" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G15" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="J15" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="M15" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="P15" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q15" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16">
@@ -1054,37 +1060,37 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="J16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="M16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N16" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="P16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q16" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17">
@@ -1092,37 +1098,37 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="J17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="M17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N17" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="P17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q17" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18">
@@ -1130,37 +1136,37 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D18" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G18" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="J18" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K18" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="M18" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N18" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="P18" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q18" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19">
@@ -1168,37 +1174,37 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D19" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G19" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="J19" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K19" t="s">
+        <v>60</v>
+      </c>
+      <c r="M19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N19" t="s">
+        <v>61</v>
+      </c>
+      <c r="P19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="s">
         <v>35</v>
-      </c>
-      <c r="M19" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="N19" t="s">
-        <v>64</v>
-      </c>
-      <c r="P19" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="20">
@@ -1206,37 +1212,37 @@
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D20" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G20" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J20" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M20" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N20" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="P20" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q20" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21">
@@ -1244,37 +1250,37 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D21" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G21" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="J21" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K21" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="M21" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N21" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="P21" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q21" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22">
@@ -1282,31 +1288,37 @@
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D22" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G22" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="J22" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K22" t="s">
-        <v>48</v>
+        <v>44</v>
+      </c>
+      <c r="M22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N22" t="s">
+        <v>42</v>
       </c>
       <c r="P22" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q22" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23">
@@ -1314,31 +1326,31 @@
         <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D23" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G23" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H23" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J23" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K23" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="P23" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q23" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24">
@@ -1346,25 +1358,31 @@
         <v>0</v>
       </c>
       <c r="B24" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D24" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>81</v>
+        <v>78</v>
+      </c>
+      <c r="G24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" t="s">
+        <v>79</v>
       </c>
       <c r="J24" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K24" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="P24" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q24" t="s">
-        <v>82</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25">
@@ -1372,25 +1390,25 @@
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="D25" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="J25" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K25" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="P25" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q25" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26">
@@ -1398,25 +1416,25 @@
         <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="D26" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="J26" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K26" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="P26" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27">
@@ -1424,25 +1442,25 @@
         <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D27" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="J27" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K27" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="P27" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q27" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28">
@@ -1450,18 +1468,24 @@
         <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D28" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="J28" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K28" t="s">
+        <v>76</v>
+      </c>
+      <c r="P28" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q28" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1470,33 +1494,39 @@
         <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D29" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E29" t="s">
+        <v>87</v>
+      </c>
+      <c r="J29" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K29" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
         <v>70</v>
       </c>
-      <c r="J29" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K29" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="D30" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E30" t="s">
-        <v>90</v>
-      </c>
       <c r="J30" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K30" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31">
@@ -1504,13 +1534,13 @@
         <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J31" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K31" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32">
@@ -1518,13 +1548,67 @@
         <v>0</v>
       </c>
       <c r="E32" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="J32" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K32" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="D33" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>39</v>
+      </c>
+      <c r="J33" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K33" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="D34" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="D35" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="D36" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="D37" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="D38" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>